<commit_message>
updated checklist and added .md file
</commit_message>
<xml_diff>
--- a/docs/QA/Basic-Testing-Checklist.xlsx
+++ b/docs/QA/Basic-Testing-Checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9A119D-A2B7-445A-B5B2-30A48D6314CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAE98A4-2700-4864-9F61-FECEEF3EEC24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,45 +29,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>1.      Minimum Input Length</t>
-  </si>
-  <si>
-    <t>2.      Maximum Input Length</t>
-  </si>
-  <si>
-    <t>3.      Accepts Special Characters</t>
-  </si>
-  <si>
-    <t>4.      Accepts Numeric/ Alpha-numeric/ Character Input respect to type of field</t>
-  </si>
-  <si>
-    <t>5.      Can user Paste  into the field</t>
-  </si>
-  <si>
-    <t>6.      Can user can Copy the field.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.      Can Delete / Edit the Text </t>
-  </si>
-  <si>
-    <t>1.      Accepts Positive Input</t>
-  </si>
-  <si>
-    <t>2.      Accepts Negative Input Values</t>
-  </si>
-  <si>
-    <t>3.      Accepts Alphabets Character Input</t>
-  </si>
-  <si>
-    <t>4.      Accepts Special Symbols</t>
-  </si>
-  <si>
-    <t>5.      Max input Length</t>
-  </si>
-  <si>
-    <t>6.      Min input Length</t>
-  </si>
-  <si>
     <t>1.      Is valid Date Pre-format shown</t>
   </si>
   <si>
@@ -233,52 +194,91 @@
     <t>General (mainly related to our application)</t>
   </si>
   <si>
-    <t>Make sure validation error messages are displayed properly at correct positions.</t>
-  </si>
-  <si>
-    <t>Check if all the error messages are displayed in the same CSS style (e.g. using red color).</t>
-  </si>
-  <si>
-    <t>Ensure general confirmation messages are displayed using CSS style (e.g. using green color) and not error messages style.</t>
-  </si>
-  <si>
-    <t>Ensure that delete functionality for any record on page is asking for confirmation.</t>
-  </si>
-  <si>
-    <t>Check text on all pages for spelling and grammatical errors.</t>
-  </si>
-  <si>
-    <t>Make sure that the scroll bar is enabled only where required.</t>
-  </si>
-  <si>
-    <t>Font size, style and color for headline, description text, labels, infield data, and grid info should be standard as specified in SRS.</t>
-  </si>
-  <si>
-    <t>Upon click of any input text field, mouse arrow pointer should get changed to cursor.</t>
-  </si>
-  <si>
-    <t>Default radio options should be pre-selected on page load.</t>
-  </si>
-  <si>
-    <t>Check all pages for broken images.</t>
-  </si>
-  <si>
-    <t>Check all pages for broken links.</t>
-  </si>
-  <si>
-    <t>Ensure that all the pages have titles.</t>
-  </si>
-  <si>
-    <t>Validate that the user is able to select only one radio option and any combination for check boxes.</t>
-  </si>
-  <si>
-    <t>Validate and ensure that all the mandatory fields are indicated by an asterisk (*) symbol.</t>
-  </si>
-  <si>
     <t>7.      File size to be confirmed.</t>
   </si>
   <si>
     <t>8.      Maximum number of Files to upload.</t>
+  </si>
+  <si>
+    <t>1. Validate and ensure that all the mandatory fields are indicated by an asterisk (*) symbol.</t>
+  </si>
+  <si>
+    <t>2. Make sure validation error messages are displayed properly at correct positions.</t>
+  </si>
+  <si>
+    <t>3. Check if all the error messages are displayed in the same CSS style (e.g. using red color).</t>
+  </si>
+  <si>
+    <t>4. Ensure general confirmation messages are displayed using CSS style (e.g. using green color) and not error messages style.</t>
+  </si>
+  <si>
+    <t>5. Ensure that delete functionality for any record on page is asking for confirmation.</t>
+  </si>
+  <si>
+    <t>6. Check text on all pages for spelling and grammatical errors.</t>
+  </si>
+  <si>
+    <t>7. Make sure that the scroll bar is enabled only where required.</t>
+  </si>
+  <si>
+    <t>8. Font size, style and color for headline, description text, labels, infield data, and grid info should be standard as specified in SRS.</t>
+  </si>
+  <si>
+    <t>9. Upon click of any input text field, mouse arrow pointer should get changed to cursor.</t>
+  </si>
+  <si>
+    <t>10. Default radio options should be pre-selected on page load.</t>
+  </si>
+  <si>
+    <t>11. Check all pages for broken images.</t>
+  </si>
+  <si>
+    <t>12. Check all pages for broken links.</t>
+  </si>
+  <si>
+    <t>13. Ensure that all the pages have titles.</t>
+  </si>
+  <si>
+    <t>14. Validate that the user is able to select only one radio option and any combination for check boxes.</t>
+  </si>
+  <si>
+    <t>1. Minimum Input Length</t>
+  </si>
+  <si>
+    <t>2. Maximum Input Length</t>
+  </si>
+  <si>
+    <t>3. Accepts Special Characters</t>
+  </si>
+  <si>
+    <t>4. Accepts Numeric/ Alpha-numeric/ Character Input respect to type of field</t>
+  </si>
+  <si>
+    <t>5. Can user Paste  into the field</t>
+  </si>
+  <si>
+    <t>6. Can user can Copy the field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Can Delete / Edit the Text </t>
+  </si>
+  <si>
+    <t>1. Accepts Positive Input</t>
+  </si>
+  <si>
+    <t>2. Accepts Negative Input Values</t>
+  </si>
+  <si>
+    <t>3. Accepts Alphabets Character Input</t>
+  </si>
+  <si>
+    <t>4. Accepts Special Symbols</t>
+  </si>
+  <si>
+    <t>5. Max input Length</t>
+  </si>
+  <si>
+    <t>6. Min input Length</t>
   </si>
 </sst>
 </file>
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.2" x14ac:dyDescent="0.35"/>
@@ -817,7 +817,7 @@
   <sheetData>
     <row r="1" spans="2:4" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="11" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -835,46 +835,46 @@
     </row>
     <row r="4" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="12" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="12"/>
       <c r="C5" s="5" t="s">
-        <v>5</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="12"/>
       <c r="C6" s="5" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="12"/>
       <c r="C7" s="5" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="12"/>
       <c r="C8" s="5" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="12"/>
       <c r="C9" s="5" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="12"/>
       <c r="C10" s="5" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -883,40 +883,40 @@
     </row>
     <row r="12" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12"/>
       <c r="C13" s="5" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12"/>
       <c r="C14" s="5" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="12"/>
       <c r="C15" s="5" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="12"/>
       <c r="C16" s="5" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="12"/>
       <c r="C17" s="5" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -925,46 +925,46 @@
     </row>
     <row r="19" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="12" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="12"/>
       <c r="C20" s="5" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B21" s="12"/>
       <c r="C21" s="5" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B22" s="12"/>
       <c r="C22" s="5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B23" s="12"/>
       <c r="C23" s="5" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B24" s="12"/>
       <c r="C24" s="5" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B25" s="12"/>
       <c r="C25" s="5" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -976,76 +976,76 @@
         <v>3</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="15"/>
       <c r="C28" s="5" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="15"/>
       <c r="C29" s="5" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="15"/>
       <c r="C30" s="5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="15"/>
       <c r="C31" s="5" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="15"/>
       <c r="C32" s="5" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="B33" s="15"/>
       <c r="C33" s="5" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="15"/>
       <c r="C34" s="5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="15"/>
       <c r="C35" s="5" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="15"/>
       <c r="C36" s="5" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="15"/>
       <c r="C37" s="5" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="15"/>
       <c r="C38" s="5" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="19.2" customHeight="1" x14ac:dyDescent="0.35">
@@ -1054,52 +1054,52 @@
     </row>
     <row r="40" spans="2:3" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="12" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41" s="12"/>
       <c r="C41" s="5" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42" s="12"/>
       <c r="C42" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43" s="12"/>
       <c r="C43" s="5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44" s="12"/>
       <c r="C44" s="5" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B45" s="12"/>
       <c r="C45" s="5" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46" s="12"/>
       <c r="C46" s="5" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47" s="12"/>
       <c r="C47" s="5" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
@@ -1108,16 +1108,16 @@
     </row>
     <row r="49" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="12" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="12"/>
       <c r="C50" s="5" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1126,34 +1126,34 @@
     </row>
     <row r="52" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B52" s="13" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="22.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B53" s="13"/>
       <c r="C53" s="5" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B54" s="13"/>
       <c r="C54" s="5" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B55" s="13"/>
       <c r="C55" s="5" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B56" s="13"/>
       <c r="C56" s="5" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1162,28 +1162,28 @@
     </row>
     <row r="58" spans="2:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B58" s="13" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B59" s="13"/>
       <c r="C59" s="5" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B60" s="13"/>
       <c r="C60" s="5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B61" s="13"/>
       <c r="C61" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
@@ -1192,153 +1192,153 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B63" s="8" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D63" s="5"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B64" s="9"/>
       <c r="C64" s="5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B65" s="9"/>
       <c r="C65" s="5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B66" s="9"/>
       <c r="C66" s="5" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" s="9"/>
       <c r="C67" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B68" s="9"/>
       <c r="C68" s="5" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B69" s="9"/>
       <c r="C69" s="5" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B70" s="10"/>
       <c r="C70" s="5" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A72" s="6"/>
       <c r="B72" s="8" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A73" s="6"/>
       <c r="B73" s="9"/>
       <c r="C73" s="7" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A74" s="6"/>
       <c r="B74" s="9"/>
       <c r="C74" s="7" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A75" s="6"/>
       <c r="B75" s="9"/>
       <c r="C75" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A76" s="6"/>
       <c r="B76" s="9"/>
       <c r="C76" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="6"/>
       <c r="B77" s="9"/>
       <c r="C77" s="7" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="6"/>
       <c r="B78" s="9"/>
       <c r="C78" s="7" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A79" s="6"/>
       <c r="B79" s="9"/>
       <c r="C79" s="7" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A80" s="6"/>
       <c r="B80" s="9"/>
       <c r="C80" s="7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="6"/>
       <c r="B81" s="9"/>
       <c r="C81" s="7" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="6"/>
       <c r="B82" s="9"/>
       <c r="C82" s="7" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="6"/>
       <c r="B83" s="9"/>
       <c r="C83" s="7" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="6"/>
       <c r="B84" s="9"/>
       <c r="C84" s="7" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="32.4" x14ac:dyDescent="0.35">
       <c r="A85" s="6"/>
       <c r="B85" s="10"/>
       <c r="C85" s="7" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>